<commit_message>
accurate analysis metrics now
</commit_message>
<xml_diff>
--- a/beta/filtered_excel_df.xlsx
+++ b/beta/filtered_excel_df.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS4"/>
+  <dimension ref="A1:AU2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -503,160 +503,170 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>fixed_resistance_gradient</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>fixed_support_gradient</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
           <t>ema_short</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>ema_long</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>lsma</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>macd_line</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>macd_signal</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>lsma_stddev</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>lsma_slope</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>prev_lsma_slope_1</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>prev_lsma_slope_2</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>lsma_upper_band</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>lsma_lower_band</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>is_buy2</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>is_sell2</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>tp</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>sl</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>be</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>be_condition</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>sl_updated</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>time_updated</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>time_to_trail</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
         <is>
           <t>time_tp_hit</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>time_sl_hit</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AL1" s="1" t="inlineStr">
         <is>
           <t>max_completion</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AM1" s="1" t="inlineStr">
         <is>
           <t>max_floating_profit</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AN1" s="1" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AO1" s="1" t="inlineStr">
         <is>
           <t>success</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AP1" s="1" t="inlineStr">
         <is>
           <t>profit</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>account_balance</t>
         </is>
       </c>
-      <c r="AP1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>win_streak</t>
         </is>
       </c>
-      <c r="AQ1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>losing_streak</t>
         </is>
       </c>
-      <c r="AR1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Week</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Month</t>
         </is>
@@ -691,389 +701,115 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>2324.03399976471</v>
+        <v>2324.033999764706</v>
       </c>
       <c r="K2" t="n">
-        <v>2331.991548581787</v>
+        <v>2331.991548581783</v>
       </c>
       <c r="L2" t="n">
-        <v>-2.422101068648088e-05</v>
+        <v>-2.422101068625785e-05</v>
       </c>
       <c r="M2" t="n">
-        <v>-6.878636050455884e-05</v>
+        <v>-6.878636050433582e-05</v>
       </c>
       <c r="N2" t="n">
+        <v>-5.833000163793168e-06</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-0.000133469848039399</v>
+      </c>
+      <c r="P2" t="n">
         <v>2328.849640934117</v>
       </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
         <v>2329.218268782417</v>
       </c>
-      <c r="P2" t="n">
+      <c r="R2" t="n">
         <v>2327.427598899206</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="S2" t="n">
         <v>-0.1464035619051174</v>
       </c>
-      <c r="R2" t="n">
+      <c r="T2" t="n">
         <v>-0.0732592765996142</v>
       </c>
-      <c r="S2" t="n">
+      <c r="U2" t="n">
         <v>2.024222649150319</v>
       </c>
-      <c r="T2" t="n">
+      <c r="V2" t="n">
         <v>-0.3529927760591818</v>
       </c>
-      <c r="U2" t="n">
+      <c r="W2" t="n">
         <v>0.04253181974308973</v>
       </c>
-      <c r="V2" t="n">
+      <c r="X2" t="n">
         <v>0.1617991056073151</v>
       </c>
-      <c r="W2" t="n">
+      <c r="Y2" t="n">
         <v>2330.160299475559</v>
       </c>
-      <c r="X2" t="n">
+      <c r="Z2" t="n">
         <v>2323.194898322854</v>
       </c>
-      <c r="Y2" t="b">
+      <c r="AA2" t="b">
         <v>0</v>
       </c>
-      <c r="Z2" t="b">
+      <c r="AB2" t="b">
         <v>1</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AC2" t="n">
         <v>2323.11</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AD2" t="n">
         <v>2330.31</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AE2" t="n">
         <v>2326.11</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AF2" t="n">
         <v>2325.91</v>
       </c>
-      <c r="AE2" t="b">
+      <c r="AG2" t="b">
         <v>0</v>
       </c>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" s="3" t="n">
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" s="3" t="n">
         <v>45462.76041666666</v>
       </c>
-      <c r="AH2" s="3" t="n">
-        <v>45464.83591435185</v>
-      </c>
-      <c r="AI2" s="3" t="n">
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" s="3" t="n">
         <v>45462.68318287037</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AL2" t="n">
         <v>48.75000000000682</v>
       </c>
-      <c r="AK2" t="n">
-        <v>70.72</v>
-      </c>
-      <c r="AL2" t="inlineStr">
+      <c r="AM2" t="n">
+        <v>70.64</v>
+      </c>
+      <c r="AN2" t="inlineStr">
         <is>
           <t>fail</t>
         </is>
       </c>
-      <c r="AM2" t="b">
+      <c r="AO2" t="b">
         <v>0</v>
       </c>
-      <c r="AN2" t="n">
-        <v>-116.09</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>183.91</v>
-      </c>
       <c r="AP2" t="n">
+        <v>-115.95</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>184.05</v>
+      </c>
+      <c r="AR2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ2" t="n">
+      <c r="AS2" t="n">
         <v>1</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="AT2" t="n">
         <v>25</v>
       </c>
-      <c r="AS2" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45463.30208333334</v>
-      </c>
-      <c r="B3" s="3" t="n">
-        <v>45463.30208333334</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2335.1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2338.37</v>
-      </c>
-      <c r="E3" t="n">
-        <v>2334.64</v>
-      </c>
-      <c r="F3" t="n">
-        <v>2338.23</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1379</v>
-      </c>
-      <c r="H3" t="n">
-        <v>27</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2334.64</v>
-      </c>
-      <c r="K3" t="n">
-        <v>2344.083577992111</v>
-      </c>
-      <c r="L3" t="n">
-        <v>0.0001147248211544992</v>
-      </c>
-      <c r="M3" t="n">
-        <v>6.452841483711299e-05</v>
-      </c>
-      <c r="N3" t="n">
-        <v>2334.424046355289</v>
-      </c>
-      <c r="O3" t="n">
-        <v>2332.871803299914</v>
-      </c>
-      <c r="P3" t="n">
-        <v>2336.212999656002</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.8152447830875644</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.68037644434393</v>
-      </c>
-      <c r="S3" t="n">
-        <v>3.070380432455432</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0.6667492260071413</v>
-      </c>
-      <c r="U3" t="n">
-        <v>0.1877227382187812</v>
-      </c>
-      <c r="V3" t="n">
-        <v>0.001224630199430976</v>
-      </c>
-      <c r="W3" t="n">
-        <v>2341.858013239817</v>
-      </c>
-      <c r="X3" t="n">
-        <v>2332.067986072188</v>
-      </c>
-      <c r="Y3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z3" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>2342.23</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>2339.23</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>2339.23</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>2339.43</v>
-      </c>
-      <c r="AE3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="3" t="n">
-        <v>45463.33333333334</v>
-      </c>
-      <c r="AG3" s="3" t="n">
-        <v>45463.33333333334</v>
-      </c>
-      <c r="AH3" s="3" t="n">
-        <v>45463.35421296296</v>
-      </c>
-      <c r="AI3" s="3" t="n">
-        <v>45463.45138888889</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>100</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>160.3</v>
-      </c>
-      <c r="AL3" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="AM3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>145.07</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>328.98</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>25</v>
-      </c>
-      <c r="AS3" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>45463.98958333334</v>
-      </c>
-      <c r="B4" s="3" t="n">
-        <v>45463.98958333334</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2358.95</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2360.06</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2358.7</v>
-      </c>
-      <c r="F4" t="n">
-        <v>2359.76</v>
-      </c>
-      <c r="G4" t="n">
-        <v>320</v>
-      </c>
-      <c r="H4" t="n">
-        <v>32</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>2357.89648758816</v>
-      </c>
-      <c r="K4" t="n">
-        <v>2360.329328111843</v>
-      </c>
-      <c r="L4" t="n">
-        <v>4.946742167959954e-05</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.0001555770177803226</v>
-      </c>
-      <c r="N4" t="n">
-        <v>2358.484907219652</v>
-      </c>
-      <c r="O4" t="n">
-        <v>2355.858187263113</v>
-      </c>
-      <c r="P4" t="n">
-        <v>2359.706845545236</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>1.893309941982807</v>
-      </c>
-      <c r="R4" t="n">
-        <v>2.089351573424988</v>
-      </c>
-      <c r="S4" t="n">
-        <v>2.563279149850003</v>
-      </c>
-      <c r="T4" t="n">
-        <v>0.1481045751634156</v>
-      </c>
-      <c r="U4" t="n">
-        <v>-0.02631922944510734</v>
-      </c>
-      <c r="V4" t="n">
-        <v>-0.04768489852131097</v>
-      </c>
-      <c r="W4" t="n">
-        <v>2364.667272397534</v>
-      </c>
-      <c r="X4" t="n">
-        <v>2356.246418692939</v>
-      </c>
-      <c r="Y4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Z4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>2363.76</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>2360.76</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>2360.76</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>2360.96</v>
-      </c>
-      <c r="AE4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="3" t="n">
-        <v>45464.13541666666</v>
-      </c>
-      <c r="AG4" s="3" t="n">
-        <v>45464.13541666666</v>
-      </c>
-      <c r="AH4" s="3" t="n">
-        <v>45464.14650462963</v>
-      </c>
-      <c r="AI4" s="3" t="n">
-        <v>45464.17711805556</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>100</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>153.05</v>
-      </c>
-      <c r="AL4" t="inlineStr">
-        <is>
-          <t>success</t>
-        </is>
-      </c>
-      <c r="AM4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>145.07</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>474.05</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>25</v>
-      </c>
-      <c r="AS4" t="n">
+      <c r="AU2" t="n">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
;atest stop loss/ tp
</commit_message>
<xml_diff>
--- a/beta/filtered_excel_df.xlsx
+++ b/beta/filtered_excel_df.xlsx
@@ -763,16 +763,16 @@
         <v>1</v>
       </c>
       <c r="AD2" t="n">
-        <v>68806.43799999999</v>
+        <v>68906.43799999999</v>
       </c>
       <c r="AE2" t="n">
-        <v>69556.43799999999</v>
+        <v>69506.43799999999</v>
       </c>
       <c r="AF2" t="n">
-        <v>69006.43799999999</v>
+        <v>69206.43799999999</v>
       </c>
       <c r="AG2" t="n">
-        <v>68906.43799999999</v>
+        <v>69156.43799999999</v>
       </c>
       <c r="AH2" t="b">
         <v>0</v>
@@ -782,16 +782,16 @@
         <v>45454.20833333334</v>
       </c>
       <c r="AK2" s="2" t="n">
-        <v>45454.20350694445</v>
+        <v>45454.20347222222</v>
       </c>
       <c r="AL2" s="2" t="n">
-        <v>45453.6125925926</v>
+        <v>45453.61202546296</v>
       </c>
       <c r="AM2" t="n">
-        <v>24.24079999999958</v>
+        <v>30.30099999999948</v>
       </c>
       <c r="AN2" t="n">
-        <v>44.71</v>
+        <v>44.02</v>
       </c>
       <c r="AO2" t="inlineStr">
         <is>
@@ -802,10 +802,10 @@
         <v>0</v>
       </c>
       <c r="AQ2" t="n">
-        <v>-92.39</v>
+        <v>-72.78</v>
       </c>
       <c r="AR2" t="n">
-        <v>207.61</v>
+        <v>377.22</v>
       </c>
       <c r="AS2" t="n">
         <v>0</v>
@@ -909,37 +909,37 @@
         <v>0</v>
       </c>
       <c r="AD3" t="n">
-        <v>70100.234</v>
+        <v>70000.234</v>
       </c>
       <c r="AE3" t="n">
-        <v>69900.234</v>
+        <v>69700.234</v>
       </c>
       <c r="AF3" t="n">
-        <v>69900.234</v>
+        <v>69700.234</v>
       </c>
       <c r="AG3" t="n">
-        <v>70000.234</v>
+        <v>69750.234</v>
       </c>
       <c r="AH3" t="b">
         <v>1</v>
       </c>
       <c r="AI3" s="2" t="n">
-        <v>45453.78125</v>
+        <v>45453.77083333334</v>
       </c>
       <c r="AJ3" s="2" t="n">
-        <v>45453.78125</v>
+        <v>45453.77083333334</v>
       </c>
       <c r="AK3" s="2" t="n">
-        <v>45453.78165509259</v>
+        <v>45453.77503472222</v>
       </c>
       <c r="AL3" s="2" t="n">
-        <v>45453.79672453704</v>
+        <v>45453.92142361111</v>
       </c>
       <c r="AM3" t="n">
         <v>100</v>
       </c>
       <c r="AN3" t="n">
-        <v>186.03</v>
+        <v>147.16</v>
       </c>
       <c r="AO3" t="inlineStr">
         <is>
@@ -950,10 +950,10 @@
         <v>1</v>
       </c>
       <c r="AQ3" t="n">
-        <v>184.73</v>
+        <v>145.52</v>
       </c>
       <c r="AR3" t="n">
-        <v>392.34</v>
+        <v>522.74</v>
       </c>
       <c r="AS3" t="n">
         <v>1</v>
@@ -1057,16 +1057,16 @@
         <v>0</v>
       </c>
       <c r="AD4" t="n">
-        <v>70552.836</v>
+        <v>70452.836</v>
       </c>
       <c r="AE4" t="n">
-        <v>69802.836</v>
+        <v>69852.836</v>
       </c>
       <c r="AF4" t="n">
-        <v>70352.836</v>
+        <v>70152.836</v>
       </c>
       <c r="AG4" t="n">
-        <v>70452.836</v>
+        <v>70202.836</v>
       </c>
       <c r="AH4" t="b">
         <v>0</v>
@@ -1075,13 +1075,13 @@
       <c r="AJ4" t="inlineStr"/>
       <c r="AK4" t="inlineStr"/>
       <c r="AL4" s="2" t="n">
-        <v>45453.89909722222</v>
+        <v>45453.89758101852</v>
       </c>
       <c r="AM4" t="n">
-        <v>18.97960000000021</v>
+        <v>23.72450000000026</v>
       </c>
       <c r="AN4" t="n">
-        <v>35.1</v>
+        <v>34.56</v>
       </c>
       <c r="AO4" t="inlineStr">
         <is>
@@ -1092,10 +1092,10 @@
         <v>0</v>
       </c>
       <c r="AQ4" t="n">
-        <v>-92.39</v>
+        <v>-72.78</v>
       </c>
       <c r="AR4" t="n">
-        <v>299.95</v>
+        <v>449.96</v>
       </c>
       <c r="AS4" t="n">
         <v>0</v>
@@ -1199,16 +1199,16 @@
         <v>1</v>
       </c>
       <c r="AD5" t="n">
-        <v>68957.93799999999</v>
+        <v>69057.93799999999</v>
       </c>
       <c r="AE5" t="n">
-        <v>69707.93799999999</v>
+        <v>69657.93799999999</v>
       </c>
       <c r="AF5" t="n">
-        <v>69157.93799999999</v>
+        <v>69357.93799999999</v>
       </c>
       <c r="AG5" t="n">
-        <v>69057.93799999999</v>
+        <v>69307.93799999999</v>
       </c>
       <c r="AH5" t="b">
         <v>0</v>
@@ -1221,13 +1221,13 @@
         <v>45454.20347222222</v>
       </c>
       <c r="AL5" s="2" t="n">
-        <v>45455.72046296296</v>
+        <v>45455.71978009259</v>
       </c>
       <c r="AM5" t="n">
         <v>100</v>
       </c>
       <c r="AN5" t="n">
-        <v>210.04</v>
+        <v>206.8</v>
       </c>
       <c r="AO5" t="inlineStr">
         <is>
@@ -1238,10 +1238,10 @@
         <v>1</v>
       </c>
       <c r="AQ5" t="n">
-        <v>184.73</v>
+        <v>145.51</v>
       </c>
       <c r="AR5" t="n">
-        <v>484.6800000000001</v>
+        <v>595.47</v>
       </c>
       <c r="AS5" t="n">
         <v>1</v>
@@ -1345,16 +1345,16 @@
         <v>1</v>
       </c>
       <c r="AD6" t="n">
-        <v>68954.734</v>
+        <v>69054.734</v>
       </c>
       <c r="AE6" t="n">
-        <v>69704.734</v>
+        <v>69654.734</v>
       </c>
       <c r="AF6" t="n">
-        <v>69154.734</v>
+        <v>69354.734</v>
       </c>
       <c r="AG6" t="n">
-        <v>69054.734</v>
+        <v>69304.734</v>
       </c>
       <c r="AH6" t="b">
         <v>0</v>
@@ -1367,13 +1367,13 @@
         <v>45454.20347222222</v>
       </c>
       <c r="AL6" s="2" t="n">
-        <v>45455.72046296296</v>
+        <v>45455.71978009259</v>
       </c>
       <c r="AM6" t="n">
         <v>100</v>
       </c>
       <c r="AN6" t="n">
-        <v>208.93</v>
+        <v>205.71</v>
       </c>
       <c r="AO6" t="inlineStr">
         <is>
@@ -1384,10 +1384,10 @@
         <v>1</v>
       </c>
       <c r="AQ6" t="n">
-        <v>184.73</v>
+        <v>145.51</v>
       </c>
       <c r="AR6" t="n">
-        <v>669.4100000000001</v>
+        <v>740.98</v>
       </c>
       <c r="AS6" t="n">
         <v>2</v>
@@ -1491,55 +1491,55 @@
         <v>1</v>
       </c>
       <c r="AD7" t="n">
-        <v>68223.234</v>
+        <v>68323.234</v>
       </c>
       <c r="AE7" t="n">
-        <v>68973.234</v>
+        <v>68923.234</v>
       </c>
       <c r="AF7" t="n">
-        <v>68423.234</v>
+        <v>68623.234</v>
       </c>
       <c r="AG7" t="n">
-        <v>68323.234</v>
+        <v>68573.234</v>
       </c>
       <c r="AH7" t="b">
         <v>0</v>
       </c>
       <c r="AI7" t="inlineStr"/>
       <c r="AJ7" s="2" t="n">
-        <v>45454.22916666666</v>
+        <v>45454.21875</v>
       </c>
       <c r="AK7" s="2" t="n">
         <v>45454.22097222223</v>
       </c>
       <c r="AL7" s="2" t="n">
-        <v>45455.64643518518</v>
+        <v>45454.21002314815</v>
       </c>
       <c r="AM7" t="n">
-        <v>100</v>
+        <v>50.45299999999771</v>
       </c>
       <c r="AN7" t="n">
-        <v>208.01</v>
+        <v>73.48</v>
       </c>
       <c r="AO7" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="AP7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ7" t="n">
-        <v>184.73</v>
+        <v>-72.77</v>
       </c>
       <c r="AR7" t="n">
-        <v>854.1400000000001</v>
+        <v>668.21</v>
       </c>
       <c r="AS7" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AT7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU7" t="n">
         <v>24</v>
@@ -1637,16 +1637,16 @@
         <v>1</v>
       </c>
       <c r="AD8" t="n">
-        <v>66431.734</v>
+        <v>66531.734</v>
       </c>
       <c r="AE8" t="n">
-        <v>67181.734</v>
+        <v>67131.734</v>
       </c>
       <c r="AF8" t="n">
-        <v>66631.734</v>
+        <v>66831.734</v>
       </c>
       <c r="AG8" t="n">
-        <v>66531.734</v>
+        <v>66781.734</v>
       </c>
       <c r="AH8" t="b">
         <v>0</v>
@@ -1656,16 +1656,16 @@
         <v>45454.78125</v>
       </c>
       <c r="AK8" s="2" t="n">
-        <v>45454.77844907407</v>
+        <v>45454.70614583333</v>
       </c>
       <c r="AL8" s="2" t="n">
-        <v>45454.67583333333</v>
+        <v>45454.63019675926</v>
       </c>
       <c r="AM8" t="n">
-        <v>27.60920000000042</v>
+        <v>32.84950000000026</v>
       </c>
       <c r="AN8" t="n">
-        <v>50.99</v>
+        <v>47.84</v>
       </c>
       <c r="AO8" t="inlineStr">
         <is>
@@ -1676,16 +1676,16 @@
         <v>0</v>
       </c>
       <c r="AQ8" t="n">
-        <v>-92.40000000000001</v>
+        <v>-72.78</v>
       </c>
       <c r="AR8" t="n">
-        <v>761.7400000000001</v>
+        <v>595.4300000000001</v>
       </c>
       <c r="AS8" t="n">
         <v>0</v>
       </c>
       <c r="AT8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AU8" t="n">
         <v>24</v>
@@ -1783,35 +1783,35 @@
         <v>1</v>
       </c>
       <c r="AD9" t="n">
-        <v>65592.883</v>
+        <v>65692.883</v>
       </c>
       <c r="AE9" t="n">
-        <v>66342.883</v>
+        <v>66292.883</v>
       </c>
       <c r="AF9" t="n">
-        <v>65792.883</v>
+        <v>65992.883</v>
       </c>
       <c r="AG9" t="n">
-        <v>65692.883</v>
+        <v>65942.883</v>
       </c>
       <c r="AH9" t="b">
         <v>0</v>
       </c>
       <c r="AI9" t="inlineStr"/>
       <c r="AJ9" s="2" t="n">
-        <v>45457.8125</v>
+        <v>45457.80208333334</v>
       </c>
       <c r="AK9" s="2" t="n">
         <v>45457.79819444445</v>
       </c>
       <c r="AL9" s="2" t="n">
-        <v>45454.78166666667</v>
+        <v>45454.78133101852</v>
       </c>
       <c r="AM9" t="n">
-        <v>4.740600000001723</v>
+        <v>5.925750000002154</v>
       </c>
       <c r="AN9" t="n">
-        <v>8.68</v>
+        <v>8.550000000000001</v>
       </c>
       <c r="AO9" t="inlineStr">
         <is>
@@ -1822,16 +1822,16 @@
         <v>0</v>
       </c>
       <c r="AQ9" t="n">
-        <v>-92.40000000000001</v>
+        <v>-72.78</v>
       </c>
       <c r="AR9" t="n">
-        <v>669.3400000000001</v>
+        <v>522.6500000000001</v>
       </c>
       <c r="AS9" t="n">
         <v>0</v>
       </c>
       <c r="AT9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AU9" t="n">
         <v>24</v>
@@ -1929,35 +1929,37 @@
         <v>0</v>
       </c>
       <c r="AD10" t="n">
-        <v>68014.234</v>
+        <v>67914.234</v>
       </c>
       <c r="AE10" t="n">
-        <v>67264.234</v>
+        <v>67614.234</v>
       </c>
       <c r="AF10" t="n">
-        <v>67814.234</v>
+        <v>67614.234</v>
       </c>
       <c r="AG10" t="n">
-        <v>67914.234</v>
+        <v>67664.234</v>
       </c>
       <c r="AH10" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI10" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AI10" s="2" t="n">
+        <v>45455.54166666666</v>
+      </c>
       <c r="AJ10" s="2" t="n">
-        <v>45455.58333333334</v>
+        <v>45455.54166666666</v>
       </c>
       <c r="AK10" s="2" t="n">
-        <v>45455.58201388889</v>
+        <v>45455.54341435185</v>
       </c>
       <c r="AL10" s="2" t="n">
-        <v>45455.95152777778</v>
+        <v>45455.94967592593</v>
       </c>
       <c r="AM10" t="n">
         <v>100</v>
       </c>
       <c r="AN10" t="n">
-        <v>187.87</v>
+        <v>154.06</v>
       </c>
       <c r="AO10" t="inlineStr">
         <is>
@@ -1968,10 +1970,10 @@
         <v>1</v>
       </c>
       <c r="AQ10" t="n">
-        <v>184.73</v>
+        <v>145.51</v>
       </c>
       <c r="AR10" t="n">
-        <v>854.0700000000002</v>
+        <v>668.1600000000001</v>
       </c>
       <c r="AS10" t="n">
         <v>1</v>
@@ -2075,16 +2077,16 @@
         <v>0</v>
       </c>
       <c r="AD11" t="n">
-        <v>69899.734</v>
+        <v>69799.734</v>
       </c>
       <c r="AE11" t="n">
-        <v>69149.734</v>
+        <v>69199.734</v>
       </c>
       <c r="AF11" t="n">
-        <v>69699.734</v>
+        <v>69499.734</v>
       </c>
       <c r="AG11" t="n">
-        <v>69799.734</v>
+        <v>69549.734</v>
       </c>
       <c r="AH11" t="b">
         <v>0</v>
@@ -2094,16 +2096,16 @@
         <v>45455.72916666666</v>
       </c>
       <c r="AK11" s="2" t="n">
-        <v>45455.72538194444</v>
+        <v>45455.72401620371</v>
       </c>
       <c r="AL11" s="2" t="n">
-        <v>45455.65880787037</v>
+        <v>45455.65797453704</v>
       </c>
       <c r="AM11" t="n">
-        <v>13.4</v>
+        <v>16.75</v>
       </c>
       <c r="AN11" t="n">
-        <v>24.75</v>
+        <v>24.37</v>
       </c>
       <c r="AO11" t="inlineStr">
         <is>
@@ -2114,10 +2116,10 @@
         <v>0</v>
       </c>
       <c r="AQ11" t="n">
-        <v>-92.39</v>
+        <v>-72.78</v>
       </c>
       <c r="AR11" t="n">
-        <v>761.6800000000002</v>
+        <v>595.3800000000001</v>
       </c>
       <c r="AS11" t="n">
         <v>0</v>
@@ -2221,37 +2223,33 @@
         <v>1</v>
       </c>
       <c r="AD12" t="n">
-        <v>68020.93799999999</v>
+        <v>68120.93799999999</v>
       </c>
       <c r="AE12" t="n">
-        <v>68220.93799999999</v>
+        <v>68720.93799999999</v>
       </c>
       <c r="AF12" t="n">
-        <v>68220.93799999999</v>
+        <v>68420.93799999999</v>
       </c>
       <c r="AG12" t="n">
-        <v>68120.93799999999</v>
+        <v>68370.93799999999</v>
       </c>
       <c r="AH12" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI12" s="2" t="n">
-        <v>45455.94791666666</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AI12" t="inlineStr"/>
       <c r="AJ12" s="2" t="n">
         <v>45455.94791666666</v>
       </c>
       <c r="AK12" s="2" t="n">
-        <v>45455.94826388889</v>
-      </c>
-      <c r="AL12" s="2" t="n">
-        <v>45455.98789351852</v>
-      </c>
+        <v>45455.94454861111</v>
+      </c>
+      <c r="AL12" t="inlineStr"/>
       <c r="AM12" t="n">
         <v>100</v>
       </c>
       <c r="AN12" t="n">
-        <v>192.31</v>
+        <v>148.42</v>
       </c>
       <c r="AO12" t="inlineStr">
         <is>
@@ -2262,10 +2260,10 @@
         <v>1</v>
       </c>
       <c r="AQ12" t="n">
-        <v>184.73</v>
+        <v>145.51</v>
       </c>
       <c r="AR12" t="n">
-        <v>946.4100000000002</v>
+        <v>740.8900000000001</v>
       </c>
       <c r="AS12" t="n">
         <v>1</v>
@@ -2369,55 +2367,55 @@
         <v>1</v>
       </c>
       <c r="AD13" t="n">
-        <v>66919.141</v>
+        <v>67019.141</v>
       </c>
       <c r="AE13" t="n">
-        <v>67669.141</v>
+        <v>67619.141</v>
       </c>
       <c r="AF13" t="n">
-        <v>67119.141</v>
+        <v>67319.141</v>
       </c>
       <c r="AG13" t="n">
-        <v>67019.141</v>
+        <v>67269.141</v>
       </c>
       <c r="AH13" t="b">
         <v>0</v>
       </c>
       <c r="AI13" t="inlineStr"/>
       <c r="AJ13" s="2" t="n">
-        <v>45456.77083333334</v>
+        <v>45456.28125</v>
       </c>
       <c r="AK13" s="2" t="n">
-        <v>45456.76706018519</v>
+        <v>45456.27650462963</v>
       </c>
       <c r="AL13" s="2" t="n">
-        <v>45456.30337962963</v>
+        <v>45456.29509259259</v>
       </c>
       <c r="AM13" t="n">
-        <v>96.06100000000151</v>
+        <v>100</v>
       </c>
       <c r="AN13" t="n">
-        <v>177.53</v>
+        <v>147.17</v>
       </c>
       <c r="AO13" t="inlineStr">
         <is>
-          <t>fail</t>
+          <t>success</t>
         </is>
       </c>
       <c r="AP13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ13" t="n">
-        <v>-92.39</v>
+        <v>145.53</v>
       </c>
       <c r="AR13" t="n">
-        <v>854.0200000000002</v>
+        <v>886.4200000000001</v>
       </c>
       <c r="AS13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU13" t="n">
         <v>24</v>
@@ -2515,35 +2513,35 @@
         <v>1</v>
       </c>
       <c r="AD14" t="n">
-        <v>66809.641</v>
+        <v>66909.641</v>
       </c>
       <c r="AE14" t="n">
-        <v>67559.641</v>
+        <v>67509.641</v>
       </c>
       <c r="AF14" t="n">
-        <v>67009.641</v>
+        <v>67209.641</v>
       </c>
       <c r="AG14" t="n">
-        <v>66909.641</v>
+        <v>67159.641</v>
       </c>
       <c r="AH14" t="b">
         <v>0</v>
       </c>
       <c r="AI14" t="inlineStr"/>
       <c r="AJ14" s="2" t="n">
-        <v>45456.78125</v>
+        <v>45456.77083333334</v>
       </c>
       <c r="AK14" s="2" t="n">
-        <v>45456.77542824074</v>
+        <v>45456.7699537037</v>
       </c>
       <c r="AL14" s="2" t="n">
-        <v>45456.34327546296</v>
+        <v>45456.33908564815</v>
       </c>
       <c r="AM14" t="n">
-        <v>1.501600000000326</v>
+        <v>1.877000000000407</v>
       </c>
       <c r="AN14" t="n">
-        <v>2.77</v>
+        <v>2.73</v>
       </c>
       <c r="AO14" t="inlineStr">
         <is>
@@ -2554,16 +2552,16 @@
         <v>0</v>
       </c>
       <c r="AQ14" t="n">
-        <v>-92.39</v>
+        <v>-72.78</v>
       </c>
       <c r="AR14" t="n">
-        <v>761.6300000000002</v>
+        <v>813.6400000000001</v>
       </c>
       <c r="AS14" t="n">
         <v>0</v>
       </c>
       <c r="AT14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AU14" t="n">
         <v>24</v>
@@ -2661,22 +2659,24 @@
         <v>0</v>
       </c>
       <c r="AD15" t="n">
-        <v>68292.43799999999</v>
+        <v>68192.43799999999</v>
       </c>
       <c r="AE15" t="n">
-        <v>67542.43799999999</v>
+        <v>67592.43799999999</v>
       </c>
       <c r="AF15" t="n">
-        <v>68092.43799999999</v>
+        <v>67892.43799999999</v>
       </c>
       <c r="AG15" t="n">
-        <v>68192.43799999999</v>
+        <v>67942.43799999999</v>
       </c>
       <c r="AH15" t="b">
         <v>0</v>
       </c>
       <c r="AI15" t="inlineStr"/>
-      <c r="AJ15" t="inlineStr"/>
+      <c r="AJ15" s="2" t="n">
+        <v>45456.6875</v>
+      </c>
       <c r="AK15" s="2" t="n">
         <v>45456.64590277777</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>100</v>
       </c>
       <c r="AN15" t="n">
-        <v>210.4</v>
+        <v>207.2</v>
       </c>
       <c r="AO15" t="inlineStr">
         <is>
@@ -2698,10 +2698,10 @@
         <v>1</v>
       </c>
       <c r="AQ15" t="n">
-        <v>184.72</v>
+        <v>145.53</v>
       </c>
       <c r="AR15" t="n">
-        <v>946.3500000000003</v>
+        <v>959.1700000000001</v>
       </c>
       <c r="AS15" t="n">
         <v>1</v>
@@ -2805,35 +2805,35 @@
         <v>1</v>
       </c>
       <c r="AD16" t="n">
-        <v>66027.836</v>
+        <v>66127.836</v>
       </c>
       <c r="AE16" t="n">
-        <v>66777.836</v>
+        <v>66727.836</v>
       </c>
       <c r="AF16" t="n">
-        <v>66227.836</v>
+        <v>66427.836</v>
       </c>
       <c r="AG16" t="n">
-        <v>66127.836</v>
+        <v>66377.836</v>
       </c>
       <c r="AH16" t="b">
         <v>0</v>
       </c>
       <c r="AI16" t="inlineStr"/>
       <c r="AJ16" s="2" t="n">
-        <v>45457.80208333334</v>
+        <v>45457.79166666666</v>
       </c>
       <c r="AK16" s="2" t="n">
-        <v>45457.79758101852</v>
+        <v>45457.79732638889</v>
       </c>
       <c r="AL16" s="2" t="n">
-        <v>45457.00414351852</v>
+        <v>45457.00275462963</v>
       </c>
       <c r="AM16" t="n">
-        <v>1.196799999999348</v>
+        <v>1.495999999999185</v>
       </c>
       <c r="AN16" t="n">
-        <v>2.22</v>
+        <v>2.18</v>
       </c>
       <c r="AO16" t="inlineStr">
         <is>
@@ -2844,10 +2844,10 @@
         <v>0</v>
       </c>
       <c r="AQ16" t="n">
-        <v>-92.39</v>
+        <v>-72.79000000000001</v>
       </c>
       <c r="AR16" t="n">
-        <v>853.9600000000003</v>
+        <v>886.3800000000001</v>
       </c>
       <c r="AS16" t="n">
         <v>0</v>
@@ -2951,31 +2951,33 @@
         <v>0</v>
       </c>
       <c r="AD17" t="n">
-        <v>67595.336</v>
+        <v>67495.336</v>
       </c>
       <c r="AE17" t="n">
-        <v>66845.336</v>
+        <v>66895.336</v>
       </c>
       <c r="AF17" t="n">
-        <v>67395.336</v>
+        <v>67195.336</v>
       </c>
       <c r="AG17" t="n">
-        <v>67495.336</v>
+        <v>67245.336</v>
       </c>
       <c r="AH17" t="b">
         <v>0</v>
       </c>
       <c r="AI17" t="inlineStr"/>
-      <c r="AJ17" t="inlineStr"/>
+      <c r="AJ17" s="2" t="n">
+        <v>45457.6875</v>
+      </c>
       <c r="AK17" t="inlineStr"/>
       <c r="AL17" s="2" t="n">
-        <v>45457.46125</v>
+        <v>45457.39572916667</v>
       </c>
       <c r="AM17" t="n">
-        <v>21.7</v>
+        <v>27.125</v>
       </c>
       <c r="AN17" t="n">
-        <v>40.09</v>
+        <v>39.47</v>
       </c>
       <c r="AO17" t="inlineStr">
         <is>
@@ -2986,10 +2988,10 @@
         <v>0</v>
       </c>
       <c r="AQ17" t="n">
-        <v>-92.39</v>
+        <v>-72.78</v>
       </c>
       <c r="AR17" t="n">
-        <v>761.5700000000003</v>
+        <v>813.6000000000001</v>
       </c>
       <c r="AS17" t="n">
         <v>0</v>
@@ -3093,16 +3095,16 @@
         <v>0</v>
       </c>
       <c r="AD18" t="n">
-        <v>67671.93799999999</v>
+        <v>67571.93799999999</v>
       </c>
       <c r="AE18" t="n">
-        <v>66921.93799999999</v>
+        <v>66971.93799999999</v>
       </c>
       <c r="AF18" t="n">
-        <v>67471.93799999999</v>
+        <v>67271.93799999999</v>
       </c>
       <c r="AG18" t="n">
-        <v>67571.93799999999</v>
+        <v>67321.93799999999</v>
       </c>
       <c r="AH18" t="b">
         <v>0</v>
@@ -3111,13 +3113,13 @@
       <c r="AJ18" t="inlineStr"/>
       <c r="AK18" t="inlineStr"/>
       <c r="AL18" s="2" t="n">
-        <v>45457.52892361111</v>
+        <v>45457.52247685185</v>
       </c>
       <c r="AM18" t="n">
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="AN18" t="n">
-        <v>18.47</v>
+        <v>18.19</v>
       </c>
       <c r="AO18" t="inlineStr">
         <is>
@@ -3128,10 +3130,10 @@
         <v>0</v>
       </c>
       <c r="AQ18" t="n">
-        <v>-92.39</v>
+        <v>-72.78</v>
       </c>
       <c r="AR18" t="n">
-        <v>669.1800000000003</v>
+        <v>740.8200000000002</v>
       </c>
       <c r="AS18" t="n">
         <v>0</v>
@@ -3235,49 +3237,51 @@
         <v>1</v>
       </c>
       <c r="AD19" t="n">
-        <v>65656.93799999999</v>
+        <v>65756.93799999999</v>
       </c>
       <c r="AE19" t="n">
-        <v>66406.93799999999</v>
+        <v>66056.93799999999</v>
       </c>
       <c r="AF19" t="n">
-        <v>65856.93799999999</v>
+        <v>66056.93799999999</v>
       </c>
       <c r="AG19" t="n">
-        <v>65756.93799999999</v>
+        <v>66006.93799999999</v>
       </c>
       <c r="AH19" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI19" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AI19" s="2" t="n">
+        <v>45460.42708333334</v>
+      </c>
       <c r="AJ19" s="2" t="n">
-        <v>45460.54166666666</v>
+        <v>45460.42708333334</v>
       </c>
       <c r="AK19" s="2" t="n">
         <v>45460.53947916667</v>
       </c>
       <c r="AL19" s="2" t="n">
-        <v>45460.85943287037</v>
+        <v>45460.43320601852</v>
       </c>
       <c r="AM19" t="n">
-        <v>100</v>
+        <v>65.01174999999785</v>
       </c>
       <c r="AN19" t="n">
-        <v>186.58</v>
+        <v>94.59</v>
       </c>
       <c r="AO19" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AP19" t="b">
         <v>1</v>
       </c>
       <c r="AQ19" t="n">
-        <v>184.73</v>
+        <v>36.38</v>
       </c>
       <c r="AR19" t="n">
-        <v>853.9100000000003</v>
+        <v>777.2000000000002</v>
       </c>
       <c r="AS19" t="n">
         <v>1</v>
@@ -3381,16 +3385,16 @@
         <v>1</v>
       </c>
       <c r="AD20" t="n">
-        <v>65625.734</v>
+        <v>65725.734</v>
       </c>
       <c r="AE20" t="n">
-        <v>66375.734</v>
+        <v>66325.734</v>
       </c>
       <c r="AF20" t="n">
-        <v>65825.734</v>
+        <v>66025.734</v>
       </c>
       <c r="AG20" t="n">
-        <v>65725.734</v>
+        <v>65975.734</v>
       </c>
       <c r="AH20" t="b">
         <v>0</v>
@@ -3400,16 +3404,16 @@
         <v>45460.54166666666</v>
       </c>
       <c r="AK20" s="2" t="n">
-        <v>45460.53949074074</v>
+        <v>45460.53947916667</v>
       </c>
       <c r="AL20" s="2" t="n">
-        <v>45460.8591087963</v>
+        <v>45460.85896990741</v>
       </c>
       <c r="AM20" t="n">
         <v>100</v>
       </c>
       <c r="AN20" t="n">
-        <v>208.19</v>
+        <v>172.44</v>
       </c>
       <c r="AO20" t="inlineStr">
         <is>
@@ -3420,10 +3424,10 @@
         <v>1</v>
       </c>
       <c r="AQ20" t="n">
-        <v>184.73</v>
+        <v>145.52</v>
       </c>
       <c r="AR20" t="n">
-        <v>1038.64</v>
+        <v>922.7200000000001</v>
       </c>
       <c r="AS20" t="n">
         <v>2</v>
@@ -3527,51 +3531,49 @@
         <v>1</v>
       </c>
       <c r="AD21" t="n">
-        <v>65481.836</v>
+        <v>65581.836</v>
       </c>
       <c r="AE21" t="n">
-        <v>65681.836</v>
+        <v>66181.836</v>
       </c>
       <c r="AF21" t="n">
-        <v>65681.836</v>
+        <v>65881.836</v>
       </c>
       <c r="AG21" t="n">
-        <v>65581.836</v>
+        <v>65831.836</v>
       </c>
       <c r="AH21" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI21" s="2" t="n">
-        <v>45460.5625</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AI21" t="inlineStr"/>
       <c r="AJ21" s="2" t="n">
-        <v>45460.5625</v>
+        <v>45460.54166666666</v>
       </c>
       <c r="AK21" s="2" t="n">
-        <v>45460.67145833333</v>
+        <v>45460.53949074074</v>
       </c>
       <c r="AL21" s="2" t="n">
-        <v>45460.56670138889</v>
+        <v>45460.85778935185</v>
       </c>
       <c r="AM21" t="n">
-        <v>87.17960000000021</v>
+        <v>100</v>
       </c>
       <c r="AN21" t="n">
-        <v>161.08</v>
+        <v>152.8</v>
       </c>
       <c r="AO21" t="inlineStr">
         <is>
-          <t>even</t>
+          <t>success</t>
         </is>
       </c>
       <c r="AP21" t="b">
         <v>1</v>
       </c>
       <c r="AQ21" t="n">
-        <v>110.84</v>
+        <v>145.52</v>
       </c>
       <c r="AR21" t="n">
-        <v>1149.48</v>
+        <v>1068.24</v>
       </c>
       <c r="AS21" t="n">
         <v>3</v>
@@ -3675,49 +3677,51 @@
         <v>1</v>
       </c>
       <c r="AD22" t="n">
-        <v>65269.859</v>
+        <v>65369.859</v>
       </c>
       <c r="AE22" t="n">
-        <v>66019.859</v>
+        <v>65669.859</v>
       </c>
       <c r="AF22" t="n">
-        <v>65469.859</v>
+        <v>65669.859</v>
       </c>
       <c r="AG22" t="n">
-        <v>65369.859</v>
+        <v>65619.859</v>
       </c>
       <c r="AH22" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI22" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AI22" s="2" t="n">
+        <v>45460.66666666666</v>
+      </c>
       <c r="AJ22" s="2" t="n">
-        <v>45460.70833333334</v>
+        <v>45460.66666666666</v>
       </c>
       <c r="AK22" s="2" t="n">
-        <v>45460.70078703704</v>
+        <v>45460.68980324074</v>
       </c>
       <c r="AL22" s="2" t="n">
-        <v>45460.82471064815</v>
+        <v>45460.67627314815</v>
       </c>
       <c r="AM22" t="n">
-        <v>100</v>
+        <v>90.5625</v>
       </c>
       <c r="AN22" t="n">
-        <v>187.68</v>
+        <v>131.87</v>
       </c>
       <c r="AO22" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AP22" t="b">
         <v>1</v>
       </c>
       <c r="AQ22" t="n">
-        <v>184.73</v>
+        <v>36.38</v>
       </c>
       <c r="AR22" t="n">
-        <v>1334.21</v>
+        <v>1104.62</v>
       </c>
       <c r="AS22" t="n">
         <v>4</v>
@@ -3821,16 +3825,16 @@
         <v>1</v>
       </c>
       <c r="AD23" t="n">
-        <v>64823.637</v>
+        <v>64923.637</v>
       </c>
       <c r="AE23" t="n">
-        <v>65573.637</v>
+        <v>65523.637</v>
       </c>
       <c r="AF23" t="n">
-        <v>65023.637</v>
+        <v>65223.637</v>
       </c>
       <c r="AG23" t="n">
-        <v>64923.637</v>
+        <v>65173.637</v>
       </c>
       <c r="AH23" t="b">
         <v>0</v>
@@ -3843,13 +3847,13 @@
         <v>45461.19717592592</v>
       </c>
       <c r="AL23" s="2" t="n">
-        <v>45460.80880787037</v>
+        <v>45460.80872685185</v>
       </c>
       <c r="AM23" t="n">
-        <v>42.59919999999984</v>
+        <v>53.24899999999979</v>
       </c>
       <c r="AN23" t="n">
-        <v>78.69</v>
+        <v>77.48999999999999</v>
       </c>
       <c r="AO23" t="inlineStr">
         <is>
@@ -3860,10 +3864,10 @@
         <v>0</v>
       </c>
       <c r="AQ23" t="n">
-        <v>-92.39</v>
+        <v>-72.78</v>
       </c>
       <c r="AR23" t="n">
-        <v>1241.82</v>
+        <v>1031.84</v>
       </c>
       <c r="AS23" t="n">
         <v>0</v>
@@ -3967,35 +3971,35 @@
         <v>1</v>
       </c>
       <c r="AD24" t="n">
-        <v>65492.836</v>
+        <v>65592.836</v>
       </c>
       <c r="AE24" t="n">
-        <v>66242.836</v>
+        <v>66192.836</v>
       </c>
       <c r="AF24" t="n">
-        <v>65692.836</v>
+        <v>65892.836</v>
       </c>
       <c r="AG24" t="n">
-        <v>65592.836</v>
+        <v>65842.836</v>
       </c>
       <c r="AH24" t="b">
         <v>0</v>
       </c>
       <c r="AI24" t="inlineStr"/>
       <c r="AJ24" s="2" t="n">
-        <v>45461.1875</v>
+        <v>45461.16666666666</v>
       </c>
       <c r="AK24" s="2" t="n">
-        <v>45461.15940972222</v>
+        <v>45461.1593287037</v>
       </c>
       <c r="AL24" s="2" t="n">
-        <v>45463.58299768518</v>
+        <v>45463.5827199074</v>
       </c>
       <c r="AM24" t="n">
         <v>100</v>
       </c>
       <c r="AN24" t="n">
-        <v>187.12</v>
+        <v>146.79</v>
       </c>
       <c r="AO24" t="inlineStr">
         <is>
@@ -4006,10 +4010,10 @@
         <v>1</v>
       </c>
       <c r="AQ24" t="n">
-        <v>184.72</v>
+        <v>145.52</v>
       </c>
       <c r="AR24" t="n">
-        <v>1426.54</v>
+        <v>1177.36</v>
       </c>
       <c r="AS24" t="n">
         <v>1</v>
@@ -4113,35 +4117,35 @@
         <v>0</v>
       </c>
       <c r="AD25" t="n">
-        <v>65911.34</v>
+        <v>65811.34</v>
       </c>
       <c r="AE25" t="n">
-        <v>65161.34</v>
+        <v>65211.34</v>
       </c>
       <c r="AF25" t="n">
-        <v>65711.34</v>
+        <v>65511.34</v>
       </c>
       <c r="AG25" t="n">
-        <v>65811.34</v>
+        <v>65561.34</v>
       </c>
       <c r="AH25" t="b">
         <v>0</v>
       </c>
       <c r="AI25" t="inlineStr"/>
       <c r="AJ25" s="2" t="n">
-        <v>45463.58333333334</v>
+        <v>45462.30208333334</v>
       </c>
       <c r="AK25" s="2" t="n">
-        <v>45463.4296412037</v>
+        <v>45463.42859953704</v>
       </c>
       <c r="AL25" s="2" t="n">
-        <v>45462.24068287037</v>
+        <v>45462.23376157408</v>
       </c>
       <c r="AM25" t="n">
-        <v>7.819600000001083</v>
+        <v>9.774500000001353</v>
       </c>
       <c r="AN25" t="n">
-        <v>14.41</v>
+        <v>14.19</v>
       </c>
       <c r="AO25" t="inlineStr">
         <is>
@@ -4152,10 +4156,10 @@
         <v>0</v>
       </c>
       <c r="AQ25" t="n">
-        <v>-92.38</v>
+        <v>-72.78</v>
       </c>
       <c r="AR25" t="n">
-        <v>1334.16</v>
+        <v>1104.58</v>
       </c>
       <c r="AS25" t="n">
         <v>0</v>
@@ -4259,55 +4263,57 @@
         <v>0</v>
       </c>
       <c r="AD26" t="n">
-        <v>65784.84</v>
+        <v>65684.84</v>
       </c>
       <c r="AE26" t="n">
-        <v>65034.84</v>
+        <v>65384.84</v>
       </c>
       <c r="AF26" t="n">
-        <v>65584.84</v>
+        <v>65384.84</v>
       </c>
       <c r="AG26" t="n">
-        <v>65684.84</v>
+        <v>65434.84</v>
       </c>
       <c r="AH26" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI26" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AI26" s="2" t="n">
+        <v>45462.28125</v>
+      </c>
       <c r="AJ26" s="2" t="n">
-        <v>45463.4375</v>
+        <v>45462.28125</v>
       </c>
       <c r="AK26" s="2" t="n">
-        <v>45463.42859953704</v>
+        <v>45462.30266203704</v>
       </c>
       <c r="AL26" s="2" t="n">
-        <v>45462.51768518519</v>
+        <v>45462.28413194444</v>
       </c>
       <c r="AM26" t="n">
-        <v>81.76020000000135</v>
+        <v>48.19925000000148</v>
       </c>
       <c r="AN26" t="n">
-        <v>151.1</v>
+        <v>70.20999999999999</v>
       </c>
       <c r="AO26" t="inlineStr">
         <is>
-          <t>fail</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AP26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ26" t="n">
-        <v>-92.38</v>
+        <v>36.38</v>
       </c>
       <c r="AR26" t="n">
-        <v>1241.78</v>
+        <v>1140.96</v>
       </c>
       <c r="AS26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT26" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AU26" t="n">
         <v>25</v>
@@ -4405,52 +4411,54 @@
         <v>0</v>
       </c>
       <c r="AD27" t="n">
-        <v>65760.34</v>
+        <v>65660.34</v>
       </c>
       <c r="AE27" t="n">
-        <v>65010.34</v>
+        <v>65360.34</v>
       </c>
       <c r="AF27" t="n">
-        <v>65560.34</v>
+        <v>65360.34</v>
       </c>
       <c r="AG27" t="n">
-        <v>65660.34</v>
+        <v>65410.34</v>
       </c>
       <c r="AH27" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI27" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AI27" s="2" t="n">
+        <v>45463.375</v>
+      </c>
       <c r="AJ27" s="2" t="n">
-        <v>45463.4375</v>
+        <v>45463.375</v>
       </c>
       <c r="AK27" s="2" t="n">
-        <v>45463.42857638889</v>
+        <v>45463.42850694444</v>
       </c>
       <c r="AL27" s="2" t="n">
-        <v>45463.70989583333</v>
+        <v>45463.4108449074</v>
       </c>
       <c r="AM27" t="n">
-        <v>100</v>
+        <v>84.84850000000006</v>
       </c>
       <c r="AN27" t="n">
-        <v>186.57</v>
+        <v>123.51</v>
       </c>
       <c r="AO27" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AP27" t="b">
         <v>1</v>
       </c>
       <c r="AQ27" t="n">
-        <v>184.72</v>
+        <v>36.38</v>
       </c>
       <c r="AR27" t="n">
-        <v>1426.5</v>
+        <v>1177.340000000001</v>
       </c>
       <c r="AS27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AT27" t="n">
         <v>0</v>
@@ -4551,52 +4559,54 @@
         <v>0</v>
       </c>
       <c r="AD28" t="n">
-        <v>65814.03899999999</v>
+        <v>65714.03899999999</v>
       </c>
       <c r="AE28" t="n">
-        <v>65064.039</v>
+        <v>65414.039</v>
       </c>
       <c r="AF28" t="n">
-        <v>65614.03899999999</v>
+        <v>65414.039</v>
       </c>
       <c r="AG28" t="n">
-        <v>65714.03899999999</v>
+        <v>65464.039</v>
       </c>
       <c r="AH28" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI28" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AI28" s="2" t="n">
+        <v>45463.375</v>
+      </c>
       <c r="AJ28" s="2" t="n">
-        <v>45463.4375</v>
+        <v>45463.375</v>
       </c>
       <c r="AK28" s="2" t="n">
-        <v>45463.42861111111</v>
+        <v>45463.42851851852</v>
       </c>
       <c r="AL28" s="2" t="n">
-        <v>45463.70924768518</v>
+        <v>45463.40783564815</v>
       </c>
       <c r="AM28" t="n">
-        <v>100</v>
+        <v>71.42375000000123</v>
       </c>
       <c r="AN28" t="n">
-        <v>185.65</v>
+        <v>103.86</v>
       </c>
       <c r="AO28" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AP28" t="b">
         <v>1</v>
       </c>
       <c r="AQ28" t="n">
-        <v>184.72</v>
+        <v>36.38</v>
       </c>
       <c r="AR28" t="n">
-        <v>1611.22</v>
+        <v>1213.720000000001</v>
       </c>
       <c r="AS28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AT28" t="n">
         <v>0</v>
@@ -4697,51 +4707,55 @@
         <v>0</v>
       </c>
       <c r="AD29" t="n">
-        <v>66665.734</v>
+        <v>66565.734</v>
       </c>
       <c r="AE29" t="n">
-        <v>65915.734</v>
+        <v>66265.734</v>
       </c>
       <c r="AF29" t="n">
-        <v>66465.734</v>
+        <v>66265.734</v>
       </c>
       <c r="AG29" t="n">
-        <v>66565.734</v>
+        <v>66315.734</v>
       </c>
       <c r="AH29" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI29" t="inlineStr"/>
-      <c r="AJ29" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AI29" s="2" t="n">
+        <v>45463.59375</v>
+      </c>
+      <c r="AJ29" s="2" t="n">
+        <v>45463.59375</v>
+      </c>
       <c r="AK29" t="inlineStr"/>
       <c r="AL29" s="2" t="n">
-        <v>45463.64006944445</v>
+        <v>45463.59940972222</v>
       </c>
       <c r="AM29" t="n">
-        <v>56.59999999999999</v>
+        <v>66.35175000000163</v>
       </c>
       <c r="AN29" t="n">
-        <v>104.55</v>
+        <v>96.59</v>
       </c>
       <c r="AO29" t="inlineStr">
         <is>
-          <t>fail</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AP29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ29" t="n">
-        <v>-92.38</v>
+        <v>36.38</v>
       </c>
       <c r="AR29" t="n">
-        <v>1518.84</v>
+        <v>1250.100000000001</v>
       </c>
       <c r="AS29" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AT29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU29" t="n">
         <v>25</v>
@@ -4839,53 +4853,55 @@
         <v>1</v>
       </c>
       <c r="AD30" t="n">
-        <v>63955.137</v>
+        <v>64055.137</v>
       </c>
       <c r="AE30" t="n">
-        <v>64705.137</v>
+        <v>64655.137</v>
       </c>
       <c r="AF30" t="n">
-        <v>64155.137</v>
+        <v>64355.137</v>
       </c>
       <c r="AG30" t="n">
-        <v>64055.137</v>
+        <v>64305.137</v>
       </c>
       <c r="AH30" t="b">
         <v>0</v>
       </c>
       <c r="AI30" t="inlineStr"/>
       <c r="AJ30" s="2" t="n">
-        <v>45464.5</v>
+        <v>45464.45833333334</v>
       </c>
       <c r="AK30" s="2" t="n">
-        <v>45464.49290509259</v>
-      </c>
-      <c r="AL30" t="inlineStr"/>
+        <v>45464.49284722222</v>
+      </c>
+      <c r="AL30" s="2" t="n">
+        <v>45464.38251157408</v>
+      </c>
       <c r="AM30" t="n">
-        <v>100</v>
+        <v>43.32425000000148</v>
       </c>
       <c r="AN30" t="n">
-        <v>186.02</v>
+        <v>63.12</v>
       </c>
       <c r="AO30" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="AP30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ30" t="n">
-        <v>184.72</v>
+        <v>-72.78</v>
       </c>
       <c r="AR30" t="n">
-        <v>1703.56</v>
+        <v>1177.320000000001</v>
       </c>
       <c r="AS30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT30" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU30" t="n">
         <v>25</v>
@@ -4983,16 +4999,16 @@
         <v>1</v>
       </c>
       <c r="AD31" t="n">
-        <v>63661.238</v>
+        <v>63761.238</v>
       </c>
       <c r="AE31" t="n">
-        <v>64411.238</v>
+        <v>64361.238</v>
       </c>
       <c r="AF31" t="n">
-        <v>63861.238</v>
+        <v>64061.238</v>
       </c>
       <c r="AG31" t="n">
-        <v>63761.238</v>
+        <v>64011.238</v>
       </c>
       <c r="AH31" t="b">
         <v>0</v>
@@ -5005,13 +5021,13 @@
         <v>45464.49291666667</v>
       </c>
       <c r="AL31" s="2" t="n">
-        <v>45464.97222222222</v>
+        <v>45464.97208333333</v>
       </c>
       <c r="AM31" t="n">
         <v>100</v>
       </c>
       <c r="AN31" t="n">
-        <v>189.52</v>
+        <v>186.63</v>
       </c>
       <c r="AO31" t="inlineStr">
         <is>
@@ -5022,13 +5038,13 @@
         <v>1</v>
       </c>
       <c r="AQ31" t="n">
-        <v>184.72</v>
+        <v>145.52</v>
       </c>
       <c r="AR31" t="n">
-        <v>1888.28</v>
+        <v>1322.840000000001</v>
       </c>
       <c r="AS31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AT31" t="n">
         <v>0</v>
@@ -5129,35 +5145,35 @@
         <v>1</v>
       </c>
       <c r="AD32" t="n">
-        <v>63093.73</v>
+        <v>63193.73</v>
       </c>
       <c r="AE32" t="n">
-        <v>63843.73</v>
+        <v>63793.73</v>
       </c>
       <c r="AF32" t="n">
-        <v>63293.73</v>
+        <v>63493.73</v>
       </c>
       <c r="AG32" t="n">
-        <v>63193.73</v>
+        <v>63443.73</v>
       </c>
       <c r="AH32" t="b">
         <v>0</v>
       </c>
       <c r="AI32" t="inlineStr"/>
       <c r="AJ32" s="2" t="n">
-        <v>45467.125</v>
+        <v>45467.11458333334</v>
       </c>
       <c r="AK32" s="2" t="n">
-        <v>45467.12850694444</v>
+        <v>45467.10893518518</v>
       </c>
       <c r="AL32" s="2" t="n">
-        <v>45464.51982638889</v>
+        <v>45464.51841435185</v>
       </c>
       <c r="AM32" t="n">
-        <v>16.6898000000001</v>
+        <v>20.86225000000013</v>
       </c>
       <c r="AN32" t="n">
-        <v>30.85</v>
+        <v>30.38</v>
       </c>
       <c r="AO32" t="inlineStr">
         <is>
@@ -5168,10 +5184,10 @@
         <v>0</v>
       </c>
       <c r="AQ32" t="n">
-        <v>-92.39</v>
+        <v>-72.78</v>
       </c>
       <c r="AR32" t="n">
-        <v>1795.89</v>
+        <v>1250.060000000001</v>
       </c>
       <c r="AS32" t="n">
         <v>0</v>
@@ -5275,49 +5291,51 @@
         <v>1</v>
       </c>
       <c r="AD33" t="n">
-        <v>63377.539</v>
+        <v>63477.539</v>
       </c>
       <c r="AE33" t="n">
-        <v>64127.539</v>
+        <v>63777.539</v>
       </c>
       <c r="AF33" t="n">
-        <v>63577.539</v>
+        <v>63777.539</v>
       </c>
       <c r="AG33" t="n">
-        <v>63477.539</v>
+        <v>63727.539</v>
       </c>
       <c r="AH33" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI33" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AI33" s="2" t="n">
+        <v>45464.61458333334</v>
+      </c>
       <c r="AJ33" s="2" t="n">
-        <v>45464.78125</v>
+        <v>45464.61458333334</v>
       </c>
       <c r="AK33" s="2" t="n">
-        <v>45464.68972222223</v>
+        <v>45464.68953703704</v>
       </c>
       <c r="AL33" s="2" t="n">
-        <v>45464.73043981481</v>
+        <v>45464.61892361111</v>
       </c>
       <c r="AM33" t="n">
-        <v>100</v>
+        <v>61.42475000000013</v>
       </c>
       <c r="AN33" t="n">
-        <v>186.2</v>
+        <v>89.31</v>
       </c>
       <c r="AO33" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AP33" t="b">
         <v>1</v>
       </c>
       <c r="AQ33" t="n">
-        <v>184.72</v>
+        <v>36.38</v>
       </c>
       <c r="AR33" t="n">
-        <v>1980.61</v>
+        <v>1286.440000000001</v>
       </c>
       <c r="AS33" t="n">
         <v>1</v>
@@ -5421,49 +5439,51 @@
         <v>1</v>
       </c>
       <c r="AD34" t="n">
-        <v>63351.84</v>
+        <v>63451.84</v>
       </c>
       <c r="AE34" t="n">
-        <v>64101.84</v>
+        <v>63751.84</v>
       </c>
       <c r="AF34" t="n">
-        <v>63551.84</v>
+        <v>63751.84</v>
       </c>
       <c r="AG34" t="n">
-        <v>63451.84</v>
+        <v>63701.84</v>
       </c>
       <c r="AH34" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI34" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AI34" s="2" t="n">
+        <v>45464.61458333334</v>
+      </c>
       <c r="AJ34" s="2" t="n">
-        <v>45467.11458333334</v>
+        <v>45464.61458333334</v>
       </c>
       <c r="AK34" s="2" t="n">
-        <v>45464.70267361111</v>
+        <v>45464.6896875</v>
       </c>
       <c r="AL34" s="2" t="n">
-        <v>45464.73038194444</v>
+        <v>45464.61849537037</v>
       </c>
       <c r="AM34" t="n">
-        <v>100</v>
+        <v>55.00000000000001</v>
       </c>
       <c r="AN34" t="n">
-        <v>186.2</v>
+        <v>80.03</v>
       </c>
       <c r="AO34" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AP34" t="b">
         <v>1</v>
       </c>
       <c r="AQ34" t="n">
-        <v>184.72</v>
+        <v>36.38</v>
       </c>
       <c r="AR34" t="n">
-        <v>2165.33</v>
+        <v>1322.820000000001</v>
       </c>
       <c r="AS34" t="n">
         <v>2</v>
@@ -5567,35 +5587,35 @@
         <v>1</v>
       </c>
       <c r="AD35" t="n">
-        <v>63096.438</v>
+        <v>63196.438</v>
       </c>
       <c r="AE35" t="n">
-        <v>63846.438</v>
+        <v>63796.438</v>
       </c>
       <c r="AF35" t="n">
-        <v>63296.438</v>
+        <v>63496.438</v>
       </c>
       <c r="AG35" t="n">
-        <v>63196.438</v>
+        <v>63446.438</v>
       </c>
       <c r="AH35" t="b">
         <v>0</v>
       </c>
       <c r="AI35" t="inlineStr"/>
       <c r="AJ35" s="2" t="n">
-        <v>45467.125</v>
+        <v>45467.11458333334</v>
       </c>
       <c r="AK35" s="2" t="n">
-        <v>45467.12849537037</v>
+        <v>45467.10893518518</v>
       </c>
       <c r="AL35" s="2" t="n">
-        <v>45464.71905092592</v>
+        <v>45464.69099537037</v>
       </c>
       <c r="AM35" t="n">
-        <v>49.70860000000103</v>
+        <v>58.32424999999967</v>
       </c>
       <c r="AN35" t="n">
-        <v>91.81</v>
+        <v>84.95</v>
       </c>
       <c r="AO35" t="inlineStr">
         <is>
@@ -5606,10 +5626,10 @@
         <v>0</v>
       </c>
       <c r="AQ35" t="n">
-        <v>-92.39</v>
+        <v>-72.78</v>
       </c>
       <c r="AR35" t="n">
-        <v>2072.94</v>
+        <v>1250.040000000001</v>
       </c>
       <c r="AS35" t="n">
         <v>0</v>
@@ -5713,53 +5733,55 @@
         <v>1</v>
       </c>
       <c r="AD36" t="n">
-        <v>62346.84</v>
+        <v>62446.84</v>
       </c>
       <c r="AE36" t="n">
-        <v>63096.84</v>
+        <v>63046.84</v>
       </c>
       <c r="AF36" t="n">
-        <v>62546.84</v>
+        <v>62746.84</v>
       </c>
       <c r="AG36" t="n">
-        <v>62446.84</v>
+        <v>62696.84</v>
       </c>
       <c r="AH36" t="b">
         <v>0</v>
       </c>
       <c r="AI36" t="inlineStr"/>
       <c r="AJ36" s="2" t="n">
-        <v>45467.36458333334</v>
+        <v>45467.30208333334</v>
       </c>
       <c r="AK36" s="2" t="n">
-        <v>45467.36094907407</v>
-      </c>
-      <c r="AL36" t="inlineStr"/>
+        <v>45467.35872685185</v>
+      </c>
+      <c r="AL36" s="2" t="n">
+        <v>45467.26145833333</v>
+      </c>
       <c r="AM36" t="n">
-        <v>100</v>
+        <v>28.75</v>
       </c>
       <c r="AN36" t="n">
-        <v>187.13</v>
+        <v>41.84</v>
       </c>
       <c r="AO36" t="inlineStr">
         <is>
-          <t>success</t>
+          <t>fail</t>
         </is>
       </c>
       <c r="AP36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ36" t="n">
-        <v>184.73</v>
+        <v>-72.78</v>
       </c>
       <c r="AR36" t="n">
-        <v>2257.67</v>
+        <v>1177.260000000001</v>
       </c>
       <c r="AS36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT36" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AU36" t="n">
         <v>26</v>
@@ -5857,55 +5879,57 @@
         <v>1</v>
       </c>
       <c r="AD37" t="n">
-        <v>62091.84</v>
+        <v>62191.84</v>
       </c>
       <c r="AE37" t="n">
-        <v>62841.84</v>
+        <v>62491.84</v>
       </c>
       <c r="AF37" t="n">
-        <v>62291.84</v>
+        <v>62491.84</v>
       </c>
       <c r="AG37" t="n">
-        <v>62191.84</v>
+        <v>62441.84</v>
       </c>
       <c r="AH37" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI37" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AI37" s="2" t="n">
+        <v>45467.36458333334</v>
+      </c>
       <c r="AJ37" s="2" t="n">
-        <v>45467.52083333334</v>
+        <v>45467.36458333334</v>
       </c>
       <c r="AK37" s="2" t="n">
-        <v>45467.51912037037</v>
+        <v>45467.37846064815</v>
       </c>
       <c r="AL37" s="2" t="n">
-        <v>45467.48403935185</v>
+        <v>45467.44347222222</v>
       </c>
       <c r="AM37" t="n">
-        <v>97.02899999999936</v>
+        <v>100</v>
       </c>
       <c r="AN37" t="n">
-        <v>179.18</v>
+        <v>146.26</v>
       </c>
       <c r="AO37" t="inlineStr">
         <is>
-          <t>fail</t>
+          <t>success</t>
         </is>
       </c>
       <c r="AP37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ37" t="n">
-        <v>-92.39</v>
+        <v>145.53</v>
       </c>
       <c r="AR37" t="n">
-        <v>2165.28</v>
+        <v>1322.790000000001</v>
       </c>
       <c r="AS37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU37" t="n">
         <v>26</v>
@@ -6003,35 +6027,35 @@
         <v>1</v>
       </c>
       <c r="AD38" t="n">
-        <v>60532.551</v>
+        <v>60632.551</v>
       </c>
       <c r="AE38" t="n">
-        <v>61282.551</v>
+        <v>61232.551</v>
       </c>
       <c r="AF38" t="n">
-        <v>60732.551</v>
+        <v>60932.551</v>
       </c>
       <c r="AG38" t="n">
-        <v>60632.551</v>
+        <v>60882.551</v>
       </c>
       <c r="AH38" t="b">
         <v>0</v>
       </c>
       <c r="AI38" t="inlineStr"/>
       <c r="AJ38" s="2" t="n">
-        <v>45467.82291666666</v>
+        <v>45467.60416666666</v>
       </c>
       <c r="AK38" s="2" t="n">
-        <v>45467.81856481481</v>
+        <v>45467.78984953704</v>
       </c>
       <c r="AL38" s="2" t="n">
-        <v>45467.53255787037</v>
+        <v>45467.53251157407</v>
       </c>
       <c r="AM38" t="n">
-        <v>6.362600000000384</v>
+        <v>7.953250000000481</v>
       </c>
       <c r="AN38" t="n">
-        <v>11.82</v>
+        <v>11.64</v>
       </c>
       <c r="AO38" t="inlineStr">
         <is>
@@ -6042,16 +6066,16 @@
         <v>0</v>
       </c>
       <c r="AQ38" t="n">
-        <v>-92.39</v>
+        <v>-72.78</v>
       </c>
       <c r="AR38" t="n">
-        <v>2072.89</v>
+        <v>1250.010000000001</v>
       </c>
       <c r="AS38" t="n">
         <v>0</v>
       </c>
       <c r="AT38" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AU38" t="n">
         <v>26</v>
@@ -6149,35 +6173,35 @@
         <v>1</v>
       </c>
       <c r="AD39" t="n">
-        <v>60006.738</v>
+        <v>60106.738</v>
       </c>
       <c r="AE39" t="n">
-        <v>60756.738</v>
+        <v>60706.738</v>
       </c>
       <c r="AF39" t="n">
-        <v>60206.738</v>
+        <v>60406.738</v>
       </c>
       <c r="AG39" t="n">
-        <v>60106.738</v>
+        <v>60356.738</v>
       </c>
       <c r="AH39" t="b">
         <v>0</v>
       </c>
       <c r="AI39" t="inlineStr"/>
       <c r="AJ39" s="2" t="n">
-        <v>45467.85416666666</v>
+        <v>45467.83333333334</v>
       </c>
       <c r="AK39" s="2" t="n">
-        <v>45467.82893518519</v>
+        <v>45467.82849537037</v>
       </c>
       <c r="AL39" s="2" t="n">
-        <v>45468.25310185185</v>
+        <v>45468.25278935185</v>
       </c>
       <c r="AM39" t="n">
         <v>100</v>
       </c>
       <c r="AN39" t="n">
-        <v>191.75</v>
+        <v>160.09</v>
       </c>
       <c r="AO39" t="inlineStr">
         <is>
@@ -6188,10 +6212,10 @@
         <v>1</v>
       </c>
       <c r="AQ39" t="n">
-        <v>184.73</v>
+        <v>145.53</v>
       </c>
       <c r="AR39" t="n">
-        <v>2257.62</v>
+        <v>1395.540000000001</v>
       </c>
       <c r="AS39" t="n">
         <v>1</v>
@@ -6295,16 +6319,16 @@
         <v>1</v>
       </c>
       <c r="AD40" t="n">
-        <v>59328.84</v>
+        <v>59428.84</v>
       </c>
       <c r="AE40" t="n">
-        <v>60078.84</v>
+        <v>60028.84</v>
       </c>
       <c r="AF40" t="n">
-        <v>59528.84</v>
+        <v>59728.84</v>
       </c>
       <c r="AG40" t="n">
-        <v>59428.84</v>
+        <v>59678.84</v>
       </c>
       <c r="AH40" t="b">
         <v>0</v>
@@ -6314,16 +6338,16 @@
         <v>45467.95833333334</v>
       </c>
       <c r="AK40" s="2" t="n">
-        <v>45467.95527777778</v>
+        <v>45467.9552662037</v>
       </c>
       <c r="AL40" s="2" t="n">
-        <v>45468.05793981482</v>
+        <v>45468.04163194444</v>
       </c>
       <c r="AM40" t="n">
         <v>100</v>
       </c>
       <c r="AN40" t="n">
-        <v>201.35</v>
+        <v>170.64</v>
       </c>
       <c r="AO40" t="inlineStr">
         <is>
@@ -6334,10 +6358,10 @@
         <v>1</v>
       </c>
       <c r="AQ40" t="n">
-        <v>184.73</v>
+        <v>145.53</v>
       </c>
       <c r="AR40" t="n">
-        <v>2442.35</v>
+        <v>1541.070000000001</v>
       </c>
       <c r="AS40" t="n">
         <v>2</v>
@@ -6441,16 +6465,16 @@
         <v>0</v>
       </c>
       <c r="AD41" t="n">
-        <v>61125.84</v>
+        <v>61025.84</v>
       </c>
       <c r="AE41" t="n">
-        <v>60375.84</v>
+        <v>60425.84</v>
       </c>
       <c r="AF41" t="n">
-        <v>60925.84</v>
+        <v>60725.84</v>
       </c>
       <c r="AG41" t="n">
-        <v>61025.84</v>
+        <v>60775.84</v>
       </c>
       <c r="AH41" t="b">
         <v>0</v>
@@ -6460,14 +6484,14 @@
         <v>45468.26041666666</v>
       </c>
       <c r="AK41" s="2" t="n">
-        <v>45468.2547337963</v>
+        <v>45468.25450231481</v>
       </c>
       <c r="AL41" t="inlineStr"/>
       <c r="AM41" t="n">
         <v>100</v>
       </c>
       <c r="AN41" t="n">
-        <v>192.48</v>
+        <v>147.72</v>
       </c>
       <c r="AO41" t="inlineStr">
         <is>
@@ -6478,10 +6502,10 @@
         <v>1</v>
       </c>
       <c r="AQ41" t="n">
-        <v>184.73</v>
+        <v>145.53</v>
       </c>
       <c r="AR41" t="n">
-        <v>2627.08</v>
+        <v>1686.600000000001</v>
       </c>
       <c r="AS41" t="n">
         <v>3</v>
@@ -6585,31 +6609,35 @@
         <v>0</v>
       </c>
       <c r="AD42" t="n">
-        <v>62539.738</v>
+        <v>62439.738</v>
       </c>
       <c r="AE42" t="n">
-        <v>61789.738</v>
+        <v>61839.738</v>
       </c>
       <c r="AF42" t="n">
-        <v>62339.738</v>
+        <v>62139.738</v>
       </c>
       <c r="AG42" t="n">
-        <v>62439.738</v>
+        <v>62189.738</v>
       </c>
       <c r="AH42" t="b">
         <v>0</v>
       </c>
       <c r="AI42" t="inlineStr"/>
-      <c r="AJ42" t="inlineStr"/>
-      <c r="AK42" t="inlineStr"/>
+      <c r="AJ42" s="2" t="n">
+        <v>45469.21875</v>
+      </c>
+      <c r="AK42" s="2" t="n">
+        <v>45469.2202662037</v>
+      </c>
       <c r="AL42" s="2" t="n">
-        <v>45468.73606481482</v>
+        <v>45468.73541666667</v>
       </c>
       <c r="AM42" t="n">
-        <v>9.6</v>
+        <v>12</v>
       </c>
       <c r="AN42" t="n">
-        <v>17.73</v>
+        <v>17.46</v>
       </c>
       <c r="AO42" t="inlineStr">
         <is>
@@ -6620,10 +6648,10 @@
         <v>0</v>
       </c>
       <c r="AQ42" t="n">
-        <v>-92.39</v>
+        <v>-72.78</v>
       </c>
       <c r="AR42" t="n">
-        <v>2534.690000000001</v>
+        <v>1613.820000000001</v>
       </c>
       <c r="AS42" t="n">
         <v>0</v>
@@ -6727,53 +6755,57 @@
         <v>0</v>
       </c>
       <c r="AD43" t="n">
-        <v>62441.637</v>
+        <v>62341.637</v>
       </c>
       <c r="AE43" t="n">
-        <v>61691.637</v>
+        <v>62041.637</v>
       </c>
       <c r="AF43" t="n">
-        <v>62241.637</v>
+        <v>62041.637</v>
       </c>
       <c r="AG43" t="n">
-        <v>62341.637</v>
+        <v>62091.637</v>
       </c>
       <c r="AH43" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI43" t="inlineStr"/>
-      <c r="AJ43" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AI43" s="2" t="n">
+        <v>45469.0625</v>
+      </c>
+      <c r="AJ43" s="2" t="n">
+        <v>45469.0625</v>
+      </c>
       <c r="AK43" s="2" t="n">
-        <v>45469.22042824074</v>
+        <v>45469.21556712963</v>
       </c>
       <c r="AL43" s="2" t="n">
-        <v>45469.09050925926</v>
+        <v>45469.06909722222</v>
       </c>
       <c r="AM43" t="n">
-        <v>36.3</v>
+        <v>43.72549999999865</v>
       </c>
       <c r="AN43" t="n">
-        <v>67.06</v>
+        <v>63.67</v>
       </c>
       <c r="AO43" t="inlineStr">
         <is>
-          <t>fail</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AP43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ43" t="n">
-        <v>-92.39</v>
+        <v>36.38</v>
       </c>
       <c r="AR43" t="n">
-        <v>2442.300000000001</v>
+        <v>1650.200000000001</v>
       </c>
       <c r="AS43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT43" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AU43" t="n">
         <v>26</v>
@@ -6871,55 +6903,57 @@
         <v>1</v>
       </c>
       <c r="AD44" t="n">
-        <v>60982.539</v>
+        <v>61082.539</v>
       </c>
       <c r="AE44" t="n">
-        <v>61732.539</v>
+        <v>61382.539</v>
       </c>
       <c r="AF44" t="n">
-        <v>61182.539</v>
+        <v>61382.539</v>
       </c>
       <c r="AG44" t="n">
-        <v>61082.539</v>
+        <v>61332.539</v>
       </c>
       <c r="AH44" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI44" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="AI44" s="2" t="n">
+        <v>45469.53125</v>
+      </c>
       <c r="AJ44" s="2" t="n">
-        <v>45469.84375</v>
+        <v>45469.53125</v>
       </c>
       <c r="AK44" s="2" t="n">
-        <v>45469.83605324074</v>
+        <v>45469.83603009259</v>
       </c>
       <c r="AL44" s="2" t="n">
-        <v>45469.69935185185</v>
+        <v>45469.5328125</v>
       </c>
       <c r="AM44" t="n">
-        <v>70.13980000000011</v>
+        <v>41.92174999999952</v>
       </c>
       <c r="AN44" t="n">
-        <v>129.49</v>
+        <v>60.94</v>
       </c>
       <c r="AO44" t="inlineStr">
         <is>
-          <t>fail</t>
+          <t>even</t>
         </is>
       </c>
       <c r="AP44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ44" t="n">
-        <v>-92.39</v>
+        <v>36.38</v>
       </c>
       <c r="AR44" t="n">
-        <v>2349.910000000001</v>
+        <v>1686.580000000001</v>
       </c>
       <c r="AS44" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT44" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AU44" t="n">
         <v>26</v>
@@ -7017,16 +7051,16 @@
         <v>1</v>
       </c>
       <c r="AD45" t="n">
-        <v>60831.84</v>
+        <v>60931.84</v>
       </c>
       <c r="AE45" t="n">
-        <v>61581.84</v>
+        <v>61531.84</v>
       </c>
       <c r="AF45" t="n">
-        <v>61031.84</v>
+        <v>61231.84</v>
       </c>
       <c r="AG45" t="n">
-        <v>60931.84</v>
+        <v>61181.84</v>
       </c>
       <c r="AH45" t="b">
         <v>0</v>
@@ -7036,16 +7070,16 @@
         <v>45469.84375</v>
       </c>
       <c r="AK45" s="2" t="n">
-        <v>45469.83891203703</v>
+        <v>45469.83692129629</v>
       </c>
       <c r="AL45" s="2" t="n">
-        <v>45469.68971064815</v>
+        <v>45469.59415509259</v>
       </c>
       <c r="AM45" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="AN45" t="n">
-        <v>73.89</v>
+        <v>72.77</v>
       </c>
       <c r="AO45" t="inlineStr">
         <is>
@@ -7056,16 +7090,16 @@
         <v>0</v>
       </c>
       <c r="AQ45" t="n">
-        <v>-92.39</v>
+        <v>-72.78</v>
       </c>
       <c r="AR45" t="n">
-        <v>2257.520000000001</v>
+        <v>1613.800000000001</v>
       </c>
       <c r="AS45" t="n">
         <v>0</v>
       </c>
       <c r="AT45" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AU45" t="n">
         <v>26</v>

</xml_diff>